<commit_message>
DOMA-1155 regenerate excel templates
</commit_message>
<xml_diff>
--- a/apps/condo/domains/meter/templates/en/MeterReadingsExportTemplate.xlsx
+++ b/apps/condo/domains/meter/templates/en/MeterReadingsExportTemplate.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -388,21 +388,33 @@
         <v>Address</v>
       </c>
       <c r="C1" t="str">
+        <v>Unit</v>
+      </c>
+      <c r="D1" t="str">
         <v>Service</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Meter number</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Place</v>
       </c>
-      <c r="F1" t="str">
-        <v>Reading</v>
-      </c>
       <c r="G1" t="str">
+        <v>Reading from tariff №1</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Reading from tariff №2</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Reading from tariff №3</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Reading from tariff №4</v>
+      </c>
+      <c r="K1" t="str">
         <v>Contact</v>
       </c>
-      <c r="H1" t="str">
+      <c r="L1" t="str">
         <v>Source</v>
       </c>
     </row>
@@ -414,21 +426,33 @@
         <v>{d.meter[i].address}</v>
       </c>
       <c r="C2" t="str">
+        <v>{d.meter[i].unitName}</v>
+      </c>
+      <c r="D2" t="str">
         <v>{d.meter[i].resource}</v>
       </c>
-      <c r="D2" t="str">
+      <c r="E2" t="str">
         <v>{d.meter[i].number}</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>{d.meter[i].place}</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>{d.meter[i].value1}</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
+        <v>{d.meter[i].value2}</v>
+      </c>
+      <c r="I2" t="str">
+        <v>{d.meter[i].value3}</v>
+      </c>
+      <c r="J2" t="str">
+        <v>{d.meter[i].value4}</v>
+      </c>
+      <c r="K2" t="str">
         <v>{d.meter[i].clientName}</v>
       </c>
-      <c r="H2" t="str">
+      <c r="L2" t="str">
         <v>{d.meter[i].source}</v>
       </c>
     </row>
@@ -440,27 +464,39 @@
         <v>{d.meter[i + 1].address}</v>
       </c>
       <c r="C3" t="str">
+        <v>{d.meter[i + 1].unitName}</v>
+      </c>
+      <c r="D3" t="str">
         <v>{d.meter[i + 1].resource}</v>
       </c>
-      <c r="D3" t="str">
+      <c r="E3" t="str">
         <v>{d.meter[i + 1].number}</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>{d.meter[i + 1].place}</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>{d.meter[i + 1].value1}</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
+        <v>{d.meter[i + 1].value2}</v>
+      </c>
+      <c r="I3" t="str">
+        <v>{d.meter[i + 1].value3}</v>
+      </c>
+      <c r="J3" t="str">
+        <v>{d.meter[i + 1].value4}</v>
+      </c>
+      <c r="K3" t="str">
         <v>{d.meter[i + 1].clientName}</v>
       </c>
-      <c r="H3" t="str">
+      <c r="L3" t="str">
         <v>{d.meter[i + 1].source}</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DOMA-1856 add account number column in export meter readings
</commit_message>
<xml_diff>
--- a/apps/condo/domains/meter/templates/en/MeterReadingsExportTemplate.xlsx
+++ b/apps/condo/domains/meter/templates/en/MeterReadingsExportTemplate.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -391,30 +391,33 @@
         <v>Unit</v>
       </c>
       <c r="D1" t="str">
+        <v>Account number</v>
+      </c>
+      <c r="E1" t="str">
         <v>Service</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Meter number</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Place</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>Reading from tariff №1</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>Reading from tariff №2</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Reading from tariff №3</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>Reading from tariff №4</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>Contact</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>Source</v>
       </c>
     </row>
@@ -429,30 +432,33 @@
         <v>{d.meter[i].unitName}</v>
       </c>
       <c r="D2" t="str">
+        <v>{d.meter[i].accountNumber}</v>
+      </c>
+      <c r="E2" t="str">
         <v>{d.meter[i].resource}</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>{d.meter[i].number}</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>{d.meter[i].place}</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>{d.meter[i].value1}</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>{d.meter[i].value2}</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>{d.meter[i].value3}</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <v>{d.meter[i].value4}</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <v>{d.meter[i].clientName}</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <v>{d.meter[i].source}</v>
       </c>
     </row>
@@ -467,36 +473,39 @@
         <v>{d.meter[i + 1].unitName}</v>
       </c>
       <c r="D3" t="str">
+        <v>{d.meter[i + 1].accountNumber}</v>
+      </c>
+      <c r="E3" t="str">
         <v>{d.meter[i + 1].resource}</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>{d.meter[i + 1].number}</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>{d.meter[i + 1].place}</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>{d.meter[i + 1].value1}</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>{d.meter[i + 1].value2}</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <v>{d.meter[i + 1].value3}</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" t="str">
         <v>{d.meter[i + 1].value4}</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <v>{d.meter[i + 1].clientName}</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <v>{d.meter[i + 1].source}</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>